<commit_message>
Changes to maps and graphics
</commit_message>
<xml_diff>
--- a/sampling/sampled_villages.xlsx
+++ b/sampling/sampled_villages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pivot_table" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </definedNames>
   <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="445">
   <si>
     <t>lz</t>
   </si>
@@ -1652,943 +1652,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="196">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-        <vertical style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </left>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </top>
-      </border>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <border>
         <top style="thin">
@@ -4900,8 +3964,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A1:I59" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A1:I81" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0">
       <items count="6">
@@ -4951,13 +4015,13 @@
         <item sd="0" x="15"/>
         <item sd="0" x="8"/>
         <item sd="0" x="9"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
         <item sd="0" x="5"/>
         <item sd="0" x="11"/>
         <item sd="0" x="17"/>
-        <item sd="0" x="1"/>
+        <item x="1"/>
         <item sd="0" x="6"/>
         <item sd="0" x="12"/>
         <item sd="0" x="18"/>
@@ -5185,7 +4249,7 @@
     <field x="9"/>
     <field x="16"/>
   </rowFields>
-  <rowItems count="56">
+  <rowItems count="78">
     <i>
       <x/>
     </i>
@@ -5249,6 +4313,12 @@
     <i r="3">
       <x v="12"/>
     </i>
+    <i r="4">
+      <x v="89"/>
+    </i>
+    <i r="5">
+      <x v="37"/>
+    </i>
     <i r="2">
       <x v="4"/>
     </i>
@@ -5264,11 +4334,71 @@
     <i r="3">
       <x v="6"/>
     </i>
+    <i r="4">
+      <x v="1"/>
+    </i>
+    <i r="5">
+      <x v="3"/>
+    </i>
+    <i r="4">
+      <x v="5"/>
+    </i>
+    <i r="5">
+      <x v="42"/>
+    </i>
+    <i r="4">
+      <x v="26"/>
+    </i>
+    <i r="5">
+      <x v="14"/>
+    </i>
+    <i r="4">
+      <x v="27"/>
+    </i>
+    <i r="5">
+      <x v="53"/>
+    </i>
+    <i r="4">
+      <x v="29"/>
+    </i>
+    <i r="5">
+      <x v="55"/>
+    </i>
     <i r="3">
       <x v="7"/>
     </i>
+    <i r="4">
+      <x v="76"/>
+    </i>
+    <i r="5">
+      <x v="32"/>
+    </i>
+    <i r="4">
+      <x v="80"/>
+    </i>
+    <i r="5">
+      <x v="33"/>
+    </i>
     <i r="3">
       <x v="8"/>
+    </i>
+    <i r="4">
+      <x v="24"/>
+    </i>
+    <i r="5">
+      <x v="51"/>
+    </i>
+    <i r="4">
+      <x v="59"/>
+    </i>
+    <i r="5">
+      <x v="26"/>
+    </i>
+    <i r="4">
+      <x v="65"/>
+    </i>
+    <i r="5">
+      <x v="28"/>
     </i>
     <i r="2">
       <x v="6"/>
@@ -5383,7 +4513,7 @@
     <i t="grand">
       <x/>
     </i>
-    <i t="grand" i="1">
+    <i t="grand">
       <x/>
     </i>
   </colItems>
@@ -5392,36 +4522,36 @@
     <dataField name="num_villages" fld="12" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="28">
-    <format dxfId="195">
+    <format dxfId="27">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="194">
+    <format dxfId="26">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="193">
+    <format dxfId="25">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="192">
+    <format dxfId="24">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="191">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="190">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="189">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="188">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5434,7 +4564,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="187">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5444,7 +4574,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="186">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5454,7 +4584,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="185">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5467,7 +4597,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="184">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5477,7 +4607,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="183">
+    <format dxfId="15">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0" defaultSubtotal="1">
@@ -5486,10 +4616,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="182">
+    <format dxfId="14">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="181">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" defaultSubtotal="1">
@@ -5498,7 +4628,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="180">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0" defaultSubtotal="1">
@@ -5507,10 +4637,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="179">
+    <format dxfId="11">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="178">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" defaultSubtotal="1">
@@ -5519,7 +4649,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="177">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0" defaultSubtotal="1">
@@ -5528,7 +4658,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="176">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0" defaultSubtotal="1">
@@ -5537,7 +4667,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="175">
+    <format dxfId="7">
       <pivotArea field="1" dataOnly="0" grandCol="1" outline="0" axis="axisCol" fieldPosition="1">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -5546,7 +4676,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="174">
+    <format dxfId="6">
       <pivotArea field="1" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="1">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -5555,7 +4685,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="173">
+    <format dxfId="5">
       <pivotArea field="1" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="1">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -5564,7 +4694,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="172">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -5573,7 +4703,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="171">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -5583,7 +4713,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="170">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -5593,7 +4723,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="169">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -5602,7 +4732,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="168">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -5950,13 +5080,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="9" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="14" customWidth="1"/>
@@ -6821,28 +5951,24 @@
       <c r="T24"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="6" t="s">
-        <v>20</v>
+      <c r="A25" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13">
-        <v>23832</v>
-      </c>
-      <c r="D25" s="13">
-        <v>11157</v>
-      </c>
+        <v>657</v>
+      </c>
+      <c r="D25" s="13"/>
       <c r="E25" s="24"/>
       <c r="F25" s="25">
-        <v>7</v>
-      </c>
-      <c r="G25" s="25">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G25" s="25"/>
       <c r="H25" s="18">
-        <v>34989</v>
+        <v>657</v>
       </c>
       <c r="I25" s="13">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J25"/>
       <c r="K25"/>
@@ -6857,12 +5983,12 @@
       <c r="T25"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="7" t="s">
-        <v>21</v>
+      <c r="A26" s="16" t="s">
+        <v>37</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13">
-        <v>1821</v>
+        <v>657</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="24"/>
@@ -6871,7 +5997,7 @@
       </c>
       <c r="G26" s="25"/>
       <c r="H26" s="18">
-        <v>1821</v>
+        <v>657</v>
       </c>
       <c r="I26" s="13">
         <v>1</v>
@@ -6889,24 +6015,28 @@
       <c r="T26"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="8" t="s">
-        <v>38</v>
+      <c r="A27" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13">
-        <v>1821</v>
-      </c>
-      <c r="D27" s="13"/>
+        <v>23832</v>
+      </c>
+      <c r="D27" s="13">
+        <v>11157</v>
+      </c>
       <c r="E27" s="24"/>
       <c r="F27" s="25">
-        <v>1</v>
-      </c>
-      <c r="G27" s="25"/>
+        <v>7</v>
+      </c>
+      <c r="G27" s="25">
+        <v>4</v>
+      </c>
       <c r="H27" s="18">
-        <v>1821</v>
+        <v>34989</v>
       </c>
       <c r="I27" s="13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J27"/>
       <c r="K27"/>
@@ -6921,8 +6051,8 @@
       <c r="T27"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="16" t="s">
-        <v>41</v>
+      <c r="A28" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13">
@@ -6953,28 +6083,24 @@
       <c r="T28"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="7" t="s">
-        <v>42</v>
+      <c r="A29" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13">
-        <v>6654</v>
-      </c>
-      <c r="D29" s="13">
-        <v>6513</v>
-      </c>
+        <v>1821</v>
+      </c>
+      <c r="D29" s="13"/>
       <c r="E29" s="24"/>
       <c r="F29" s="25">
-        <v>2</v>
-      </c>
-      <c r="G29" s="25">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G29" s="25"/>
       <c r="H29" s="18">
-        <v>13167</v>
+        <v>1821</v>
       </c>
       <c r="I29" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J29"/>
       <c r="K29"/>
@@ -6989,24 +6115,24 @@
       <c r="T29"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="7" t="s">
-        <v>63</v>
+      <c r="A30" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13">
-        <v>3582</v>
+        <v>1821</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="24"/>
       <c r="F30" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" s="25"/>
       <c r="H30" s="18">
-        <v>3582</v>
+        <v>1821</v>
       </c>
       <c r="I30" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30"/>
       <c r="K30"/>
@@ -7022,27 +6148,27 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="7" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13">
-        <v>11775</v>
+        <v>6654</v>
       </c>
       <c r="D31" s="13">
-        <v>4644</v>
+        <v>6513</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="25">
         <v>2</v>
       </c>
       <c r="G31" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H31" s="18">
-        <v>16419</v>
+        <v>13167</v>
       </c>
       <c r="I31" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J31"/>
       <c r="K31"/>
@@ -7057,28 +6183,24 @@
       <c r="T31"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="6" t="s">
-        <v>85</v>
+      <c r="A32" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13">
-        <v>33714</v>
-      </c>
-      <c r="D32" s="13">
-        <v>2712</v>
-      </c>
+        <v>2208</v>
+      </c>
+      <c r="D32" s="13"/>
       <c r="E32" s="24"/>
       <c r="F32" s="25">
-        <v>7</v>
-      </c>
-      <c r="G32" s="25">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G32" s="25"/>
       <c r="H32" s="18">
-        <v>36426</v>
+        <v>2208</v>
       </c>
       <c r="I32" s="13">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J32"/>
       <c r="K32"/>
@@ -7093,28 +6215,24 @@
       <c r="T32"/>
     </row>
     <row r="33" spans="1:20">
-      <c r="A33" s="7" t="s">
-        <v>86</v>
+      <c r="A33" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13">
-        <v>21552</v>
-      </c>
-      <c r="D33" s="13">
-        <v>1665</v>
-      </c>
+        <v>2208</v>
+      </c>
+      <c r="D33" s="13"/>
       <c r="E33" s="24"/>
       <c r="F33" s="25">
-        <v>3</v>
-      </c>
-      <c r="G33" s="25">
         <v>1</v>
       </c>
+      <c r="G33" s="25"/>
       <c r="H33" s="18">
-        <v>23217</v>
+        <v>2208</v>
       </c>
       <c r="I33" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J33"/>
       <c r="K33"/>
@@ -7129,28 +6247,24 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:20">
-      <c r="A34" s="7" t="s">
-        <v>102</v>
+      <c r="A34" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B34" s="13"/>
-      <c r="C34" s="13">
-        <v>2793</v>
-      </c>
+      <c r="C34" s="13"/>
       <c r="D34" s="13">
-        <v>1047</v>
+        <v>1485</v>
       </c>
       <c r="E34" s="24"/>
-      <c r="F34" s="25">
-        <v>1</v>
-      </c>
+      <c r="F34" s="25"/>
       <c r="G34" s="25">
         <v>1</v>
       </c>
       <c r="H34" s="18">
-        <v>3840</v>
+        <v>1485</v>
       </c>
       <c r="I34" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J34"/>
       <c r="K34"/>
@@ -7165,24 +6279,24 @@
       <c r="T34"/>
     </row>
     <row r="35" spans="1:20">
-      <c r="A35" s="7" t="s">
-        <v>111</v>
+      <c r="A35" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="B35" s="13"/>
-      <c r="C35" s="13">
-        <v>9369</v>
-      </c>
-      <c r="D35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13">
+        <v>1485</v>
+      </c>
       <c r="E35" s="24"/>
-      <c r="F35" s="25">
-        <v>3</v>
-      </c>
-      <c r="G35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25">
+        <v>1</v>
+      </c>
       <c r="H35" s="18">
-        <v>9369</v>
+        <v>1485</v>
       </c>
       <c r="I35" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J35"/>
       <c r="K35"/>
@@ -7197,32 +6311,24 @@
       <c r="T35"/>
     </row>
     <row r="36" spans="1:20">
-      <c r="A36" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B36" s="13">
-        <v>777</v>
-      </c>
+      <c r="A36" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="13"/>
       <c r="C36" s="13">
-        <v>23787</v>
-      </c>
-      <c r="D36" s="13">
-        <v>33162</v>
-      </c>
-      <c r="E36" s="24">
+        <v>4446</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="25">
         <v>1</v>
       </c>
-      <c r="F36" s="25">
-        <v>4</v>
-      </c>
-      <c r="G36" s="25">
-        <v>5</v>
-      </c>
+      <c r="G36" s="25"/>
       <c r="H36" s="18">
-        <v>57726</v>
+        <v>4446</v>
       </c>
       <c r="I36" s="13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J36"/>
       <c r="K36"/>
@@ -7237,32 +6343,24 @@
       <c r="T36"/>
     </row>
     <row r="37" spans="1:20">
-      <c r="A37" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" s="13">
-        <v>777</v>
-      </c>
+      <c r="A37" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="13"/>
       <c r="C37" s="13">
-        <v>23787</v>
-      </c>
-      <c r="D37" s="13">
-        <v>33162</v>
-      </c>
-      <c r="E37" s="24">
+        <v>4446</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="25">
         <v>1</v>
       </c>
-      <c r="F37" s="25">
-        <v>4</v>
-      </c>
-      <c r="G37" s="25">
-        <v>5</v>
-      </c>
+      <c r="G37" s="25"/>
       <c r="H37" s="18">
-        <v>57726</v>
+        <v>4446</v>
       </c>
       <c r="I37" s="13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J37"/>
       <c r="K37"/>
@@ -7277,28 +6375,24 @@
       <c r="T37"/>
     </row>
     <row r="38" spans="1:20">
-      <c r="A38" s="7" t="s">
-        <v>168</v>
+      <c r="A38" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B38" s="13"/>
-      <c r="C38" s="13">
-        <v>21345</v>
-      </c>
+      <c r="C38" s="13"/>
       <c r="D38" s="13">
-        <v>13086</v>
+        <v>1035</v>
       </c>
       <c r="E38" s="24"/>
-      <c r="F38" s="25">
-        <v>3</v>
-      </c>
+      <c r="F38" s="25"/>
       <c r="G38" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H38" s="18">
-        <v>34431</v>
+        <v>1035</v>
       </c>
       <c r="I38" s="13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J38"/>
       <c r="K38"/>
@@ -7313,21 +6407,21 @@
       <c r="T38"/>
     </row>
     <row r="39" spans="1:20">
-      <c r="A39" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B39" s="13">
-        <v>777</v>
-      </c>
+      <c r="A39" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="13"/>
       <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="24">
+      <c r="D39" s="13">
+        <v>1035</v>
+      </c>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25">
         <v>1</v>
       </c>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
       <c r="H39" s="18">
-        <v>777</v>
+        <v>1035</v>
       </c>
       <c r="I39" s="13">
         <v>1</v>
@@ -7345,28 +6439,24 @@
       <c r="T39"/>
     </row>
     <row r="40" spans="1:20">
-      <c r="A40" s="7" t="s">
-        <v>230</v>
+      <c r="A40" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="13">
-        <v>2442</v>
-      </c>
+      <c r="C40" s="13"/>
       <c r="D40" s="13">
-        <v>20076</v>
+        <v>3993</v>
       </c>
       <c r="E40" s="24"/>
-      <c r="F40" s="25">
+      <c r="F40" s="25"/>
+      <c r="G40" s="25">
         <v>1</v>
       </c>
-      <c r="G40" s="25">
-        <v>2</v>
-      </c>
       <c r="H40" s="18">
-        <v>22518</v>
+        <v>3993</v>
       </c>
       <c r="I40" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J40"/>
       <c r="K40"/>
@@ -7381,28 +6471,24 @@
       <c r="T40"/>
     </row>
     <row r="41" spans="1:20">
-      <c r="A41" s="17" t="s">
-        <v>124</v>
+      <c r="A41" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="B41" s="13"/>
-      <c r="C41" s="13">
-        <v>18426</v>
-      </c>
+      <c r="C41" s="13"/>
       <c r="D41" s="13">
-        <v>75972</v>
+        <v>3993</v>
       </c>
       <c r="E41" s="24"/>
-      <c r="F41" s="25">
-        <v>4</v>
-      </c>
+      <c r="F41" s="25"/>
       <c r="G41" s="25">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H41" s="18">
-        <v>94398</v>
+        <v>3993</v>
       </c>
       <c r="I41" s="13">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="J41"/>
       <c r="K41"/>
@@ -7417,24 +6503,24 @@
       <c r="T41"/>
     </row>
     <row r="42" spans="1:20">
-      <c r="A42" s="5" t="s">
-        <v>19</v>
+      <c r="A42" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13">
-        <v>21006</v>
-      </c>
+      <c r="C42" s="13">
+        <v>3582</v>
+      </c>
+      <c r="D42" s="13"/>
       <c r="E42" s="24"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25">
-        <v>4</v>
-      </c>
+      <c r="F42" s="25">
+        <v>2</v>
+      </c>
+      <c r="G42" s="25"/>
       <c r="H42" s="18">
-        <v>21006</v>
+        <v>3582</v>
       </c>
       <c r="I42" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
@@ -7449,24 +6535,24 @@
       <c r="T42"/>
     </row>
     <row r="43" spans="1:20">
-      <c r="A43" s="6" t="s">
-        <v>125</v>
+      <c r="A43" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13">
-        <v>21006</v>
-      </c>
+      <c r="C43" s="13">
+        <v>2610</v>
+      </c>
+      <c r="D43" s="13"/>
       <c r="E43" s="24"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25">
-        <v>4</v>
-      </c>
+      <c r="F43" s="25">
+        <v>1</v>
+      </c>
+      <c r="G43" s="25"/>
       <c r="H43" s="18">
-        <v>21006</v>
+        <v>2610</v>
       </c>
       <c r="I43" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J43"/>
       <c r="K43"/>
@@ -7481,24 +6567,24 @@
       <c r="T43"/>
     </row>
     <row r="44" spans="1:20">
-      <c r="A44" s="7" t="s">
-        <v>126</v>
+      <c r="A44" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13">
-        <v>17196</v>
-      </c>
+      <c r="C44" s="13">
+        <v>2610</v>
+      </c>
+      <c r="D44" s="13"/>
       <c r="E44" s="24"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25">
-        <v>3</v>
-      </c>
+      <c r="F44" s="25">
+        <v>1</v>
+      </c>
+      <c r="G44" s="25"/>
       <c r="H44" s="18">
-        <v>17196</v>
+        <v>2610</v>
       </c>
       <c r="I44" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J44"/>
       <c r="K44"/>
@@ -7513,21 +6599,21 @@
       <c r="T44"/>
     </row>
     <row r="45" spans="1:20">
-      <c r="A45" s="7" t="s">
-        <v>139</v>
+      <c r="A45" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13">
-        <v>3810</v>
-      </c>
+      <c r="C45" s="13">
+        <v>972</v>
+      </c>
+      <c r="D45" s="13"/>
       <c r="E45" s="24"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25">
+      <c r="F45" s="25">
         <v>1</v>
       </c>
+      <c r="G45" s="25"/>
       <c r="H45" s="18">
-        <v>3810</v>
+        <v>972</v>
       </c>
       <c r="I45" s="13">
         <v>1</v>
@@ -7545,28 +6631,24 @@
       <c r="T45"/>
     </row>
     <row r="46" spans="1:20">
-      <c r="A46" s="5" t="s">
-        <v>166</v>
+      <c r="A46" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="B46" s="13"/>
       <c r="C46" s="13">
-        <v>18426</v>
-      </c>
-      <c r="D46" s="13">
-        <v>54966</v>
-      </c>
+        <v>972</v>
+      </c>
+      <c r="D46" s="13"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25">
-        <v>4</v>
-      </c>
-      <c r="G46" s="25">
-        <v>8</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G46" s="25"/>
       <c r="H46" s="18">
-        <v>73392</v>
+        <v>972</v>
       </c>
       <c r="I46" s="13">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J46"/>
       <c r="K46"/>
@@ -7581,28 +6663,28 @@
       <c r="T46"/>
     </row>
     <row r="47" spans="1:20">
-      <c r="A47" s="6" t="s">
-        <v>349</v>
+      <c r="A47" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="B47" s="13"/>
       <c r="C47" s="13">
-        <v>18426</v>
+        <v>11775</v>
       </c>
       <c r="D47" s="13">
-        <v>54966</v>
+        <v>4644</v>
       </c>
       <c r="E47" s="24"/>
       <c r="F47" s="25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G47" s="25">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H47" s="18">
-        <v>73392</v>
+        <v>16419</v>
       </c>
       <c r="I47" s="13">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="J47"/>
       <c r="K47"/>
@@ -7617,28 +6699,24 @@
       <c r="T47"/>
     </row>
     <row r="48" spans="1:20">
-      <c r="A48" s="7" t="s">
-        <v>350</v>
+      <c r="A48" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="B48" s="13"/>
-      <c r="C48" s="13">
-        <v>9552</v>
-      </c>
+      <c r="C48" s="13"/>
       <c r="D48" s="13">
-        <v>33306</v>
+        <v>4644</v>
       </c>
       <c r="E48" s="24"/>
-      <c r="F48" s="25">
-        <v>2</v>
-      </c>
+      <c r="F48" s="25"/>
       <c r="G48" s="25">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H48" s="18">
-        <v>42858</v>
+        <v>4644</v>
       </c>
       <c r="I48" s="13">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J48"/>
       <c r="K48"/>
@@ -7653,28 +6731,24 @@
       <c r="T48"/>
     </row>
     <row r="49" spans="1:20">
-      <c r="A49" s="7" t="s">
-        <v>383</v>
+      <c r="A49" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="B49" s="13"/>
-      <c r="C49" s="13">
-        <v>8874</v>
-      </c>
+      <c r="C49" s="13"/>
       <c r="D49" s="13">
-        <v>21660</v>
+        <v>4644</v>
       </c>
       <c r="E49" s="24"/>
-      <c r="F49" s="25">
-        <v>2</v>
-      </c>
+      <c r="F49" s="25"/>
       <c r="G49" s="25">
         <v>1</v>
       </c>
       <c r="H49" s="18">
-        <v>30534</v>
+        <v>4644</v>
       </c>
       <c r="I49" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J49"/>
       <c r="K49"/>
@@ -7689,32 +6763,24 @@
       <c r="T49"/>
     </row>
     <row r="50" spans="1:20">
-      <c r="A50" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" s="13">
-        <v>6732</v>
-      </c>
+      <c r="A50" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="13"/>
       <c r="C50" s="13">
-        <v>7413</v>
-      </c>
-      <c r="D50" s="13">
-        <v>74589</v>
-      </c>
-      <c r="E50" s="24">
-        <v>3</v>
-      </c>
+        <v>4824</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="24"/>
       <c r="F50" s="25">
-        <v>2</v>
-      </c>
-      <c r="G50" s="25">
-        <v>9</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G50" s="25"/>
       <c r="H50" s="18">
-        <v>88734</v>
+        <v>4824</v>
       </c>
       <c r="I50" s="13">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J50"/>
       <c r="K50"/>
@@ -7729,28 +6795,24 @@
       <c r="T50"/>
     </row>
     <row r="51" spans="1:20">
-      <c r="A51" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="13">
-        <v>4047</v>
-      </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13">
-        <v>14445</v>
-      </c>
-      <c r="E51" s="24">
+      <c r="A51" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13">
+        <v>4824</v>
+      </c>
+      <c r="D51" s="13"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="25">
         <v>1</v>
       </c>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25">
-        <v>4</v>
-      </c>
+      <c r="G51" s="25"/>
       <c r="H51" s="18">
-        <v>18492</v>
+        <v>4824</v>
       </c>
       <c r="I51" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J51"/>
       <c r="K51"/>
@@ -7765,28 +6827,24 @@
       <c r="T51"/>
     </row>
     <row r="52" spans="1:20">
-      <c r="A52" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B52" s="13">
-        <v>4047</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13">
-        <v>14445</v>
-      </c>
-      <c r="E52" s="24">
+      <c r="A52" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13">
+        <v>6951</v>
+      </c>
+      <c r="D52" s="13"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="25">
         <v>1</v>
       </c>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25">
-        <v>4</v>
-      </c>
+      <c r="G52" s="25"/>
       <c r="H52" s="18">
-        <v>18492</v>
+        <v>6951</v>
       </c>
       <c r="I52" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J52"/>
       <c r="K52"/>
@@ -7801,28 +6859,24 @@
       <c r="T52"/>
     </row>
     <row r="53" spans="1:20">
-      <c r="A53" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B53" s="13">
-        <v>4047</v>
-      </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13">
-        <v>14445</v>
-      </c>
-      <c r="E53" s="24">
+      <c r="A53" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13">
+        <v>6951</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="25">
         <v>1</v>
       </c>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25">
-        <v>4</v>
-      </c>
+      <c r="G53" s="25"/>
       <c r="H53" s="18">
-        <v>18492</v>
+        <v>6951</v>
       </c>
       <c r="I53" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J53"/>
       <c r="K53"/>
@@ -7837,29 +6891,25 @@
       <c r="T53"/>
     </row>
     <row r="54" spans="1:20">
-      <c r="A54" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B54" s="13">
-        <v>2685</v>
-      </c>
+      <c r="A54" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="13"/>
       <c r="C54" s="13">
-        <v>7413</v>
+        <v>33714</v>
       </c>
       <c r="D54" s="13">
-        <v>60144</v>
-      </c>
-      <c r="E54" s="24">
+        <v>2712</v>
+      </c>
+      <c r="E54" s="24"/>
+      <c r="F54" s="25">
+        <v>7</v>
+      </c>
+      <c r="G54" s="25">
         <v>2</v>
       </c>
-      <c r="F54" s="25">
-        <v>2</v>
-      </c>
-      <c r="G54" s="25">
-        <v>5</v>
-      </c>
       <c r="H54" s="18">
-        <v>70242</v>
+        <v>36426</v>
       </c>
       <c r="I54" s="13">
         <v>9</v>
@@ -7877,25 +6927,25 @@
       <c r="T54"/>
     </row>
     <row r="55" spans="1:20">
-      <c r="A55" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="B55" s="13">
-        <v>2685</v>
-      </c>
-      <c r="C55" s="13"/>
+      <c r="A55" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13">
+        <v>21552</v>
+      </c>
       <c r="D55" s="13">
-        <v>38193</v>
-      </c>
-      <c r="E55" s="24">
-        <v>2</v>
-      </c>
-      <c r="F55" s="25"/>
+        <v>1665</v>
+      </c>
+      <c r="E55" s="24"/>
+      <c r="F55" s="25">
+        <v>3</v>
+      </c>
       <c r="G55" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H55" s="18">
-        <v>40878</v>
+        <v>23217</v>
       </c>
       <c r="I55" s="13">
         <v>4</v>
@@ -7913,28 +6963,28 @@
       <c r="T55"/>
     </row>
     <row r="56" spans="1:20">
-      <c r="A56" s="6" t="s">
-        <v>349</v>
+      <c r="A56" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="B56" s="13"/>
       <c r="C56" s="13">
-        <v>7413</v>
+        <v>2793</v>
       </c>
       <c r="D56" s="13">
-        <v>21951</v>
+        <v>1047</v>
       </c>
       <c r="E56" s="24"/>
       <c r="F56" s="25">
+        <v>1</v>
+      </c>
+      <c r="G56" s="25">
+        <v>1</v>
+      </c>
+      <c r="H56" s="18">
+        <v>3840</v>
+      </c>
+      <c r="I56" s="13">
         <v>2</v>
-      </c>
-      <c r="G56" s="25">
-        <v>3</v>
-      </c>
-      <c r="H56" s="18">
-        <v>29364</v>
-      </c>
-      <c r="I56" s="13">
-        <v>5</v>
       </c>
       <c r="J56"/>
       <c r="K56"/>
@@ -7950,27 +7000,23 @@
     </row>
     <row r="57" spans="1:20">
       <c r="A57" s="7" t="s">
-        <v>350</v>
+        <v>111</v>
       </c>
       <c r="B57" s="13"/>
       <c r="C57" s="13">
-        <v>3633</v>
-      </c>
-      <c r="D57" s="13">
-        <v>21951</v>
-      </c>
+        <v>9369</v>
+      </c>
+      <c r="D57" s="13"/>
       <c r="E57" s="24"/>
       <c r="F57" s="25">
-        <v>1</v>
-      </c>
-      <c r="G57" s="25">
         <v>3</v>
       </c>
+      <c r="G57" s="25"/>
       <c r="H57" s="18">
-        <v>25584</v>
+        <v>9369</v>
       </c>
       <c r="I57" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J57"/>
       <c r="K57"/>
@@ -7985,24 +7031,32 @@
       <c r="T57"/>
     </row>
     <row r="58" spans="1:20">
-      <c r="A58" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="B58" s="13"/>
+      <c r="A58" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="13">
+        <v>777</v>
+      </c>
       <c r="C58" s="13">
-        <v>3780</v>
-      </c>
-      <c r="D58" s="13"/>
-      <c r="E58" s="24"/>
+        <v>23787</v>
+      </c>
+      <c r="D58" s="13">
+        <v>33162</v>
+      </c>
+      <c r="E58" s="24">
+        <v>1</v>
+      </c>
       <c r="F58" s="25">
-        <v>1</v>
-      </c>
-      <c r="G58" s="25"/>
+        <v>4</v>
+      </c>
+      <c r="G58" s="25">
+        <v>5</v>
+      </c>
       <c r="H58" s="18">
-        <v>3780</v>
+        <v>57726</v>
       </c>
       <c r="I58" s="13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J58"/>
       <c r="K58"/>
@@ -8017,32 +7071,32 @@
       <c r="T58"/>
     </row>
     <row r="59" spans="1:20">
-      <c r="A59" s="4" t="s">
-        <v>424</v>
+      <c r="A59" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="B59" s="13">
-        <v>10023</v>
+        <v>777</v>
       </c>
       <c r="C59" s="13">
-        <v>169950</v>
+        <v>23787</v>
       </c>
       <c r="D59" s="13">
-        <v>337206</v>
+        <v>33162</v>
       </c>
       <c r="E59" s="24">
+        <v>1</v>
+      </c>
+      <c r="F59" s="25">
+        <v>4</v>
+      </c>
+      <c r="G59" s="25">
         <v>5</v>
       </c>
-      <c r="F59" s="25">
-        <v>37</v>
-      </c>
-      <c r="G59" s="25">
-        <v>55</v>
-      </c>
       <c r="H59" s="18">
-        <v>517179</v>
+        <v>57726</v>
       </c>
       <c r="I59" s="13">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="J59"/>
       <c r="K59"/>
@@ -8057,14 +7111,29 @@
       <c r="T59"/>
     </row>
     <row r="60" spans="1:20">
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
+      <c r="A60" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13">
+        <v>21345</v>
+      </c>
+      <c r="D60" s="13">
+        <v>13086</v>
+      </c>
+      <c r="E60" s="24"/>
+      <c r="F60" s="25">
+        <v>3</v>
+      </c>
+      <c r="G60" s="25">
+        <v>3</v>
+      </c>
+      <c r="H60" s="18">
+        <v>34431</v>
+      </c>
+      <c r="I60" s="13">
+        <v>6</v>
+      </c>
       <c r="J60"/>
       <c r="K60"/>
       <c r="L60"/>
@@ -8078,14 +7147,25 @@
       <c r="T60"/>
     </row>
     <row r="61" spans="1:20">
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
+      <c r="A61" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" s="13">
+        <v>777</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="24">
+        <v>1</v>
+      </c>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="18">
+        <v>777</v>
+      </c>
+      <c r="I61" s="13">
+        <v>1</v>
+      </c>
       <c r="J61"/>
       <c r="K61"/>
       <c r="L61"/>
@@ -8099,14 +7179,29 @@
       <c r="T61"/>
     </row>
     <row r="62" spans="1:20">
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
+      <c r="A62" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13">
+        <v>2442</v>
+      </c>
+      <c r="D62" s="13">
+        <v>20076</v>
+      </c>
+      <c r="E62" s="24"/>
+      <c r="F62" s="25">
+        <v>1</v>
+      </c>
+      <c r="G62" s="25">
+        <v>2</v>
+      </c>
+      <c r="H62" s="18">
+        <v>22518</v>
+      </c>
+      <c r="I62" s="13">
+        <v>3</v>
+      </c>
       <c r="J62"/>
       <c r="K62"/>
       <c r="L62"/>
@@ -8120,14 +7215,29 @@
       <c r="T62"/>
     </row>
     <row r="63" spans="1:20">
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
+      <c r="A63" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13">
+        <v>18426</v>
+      </c>
+      <c r="D63" s="13">
+        <v>75972</v>
+      </c>
+      <c r="E63" s="24"/>
+      <c r="F63" s="25">
+        <v>4</v>
+      </c>
+      <c r="G63" s="25">
+        <v>12</v>
+      </c>
+      <c r="H63" s="18">
+        <v>94398</v>
+      </c>
+      <c r="I63" s="13">
+        <v>16</v>
+      </c>
       <c r="J63"/>
       <c r="K63"/>
       <c r="L63"/>
@@ -8141,14 +7251,25 @@
       <c r="T63"/>
     </row>
     <row r="64" spans="1:20">
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
+      <c r="A64" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13">
+        <v>21006</v>
+      </c>
+      <c r="E64" s="24"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25">
+        <v>4</v>
+      </c>
+      <c r="H64" s="18">
+        <v>21006</v>
+      </c>
+      <c r="I64" s="13">
+        <v>4</v>
+      </c>
       <c r="J64"/>
       <c r="K64"/>
       <c r="L64"/>
@@ -8161,15 +7282,26 @@
       <c r="S64"/>
       <c r="T64"/>
     </row>
-    <row r="65" spans="2:20">
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
+    <row r="65" spans="1:20">
+      <c r="A65" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13">
+        <v>21006</v>
+      </c>
+      <c r="E65" s="24"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25">
+        <v>4</v>
+      </c>
+      <c r="H65" s="18">
+        <v>21006</v>
+      </c>
+      <c r="I65" s="13">
+        <v>4</v>
+      </c>
       <c r="J65"/>
       <c r="K65"/>
       <c r="L65"/>
@@ -8182,15 +7314,26 @@
       <c r="S65"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="2:20">
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
+    <row r="66" spans="1:20">
+      <c r="A66" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13">
+        <v>17196</v>
+      </c>
+      <c r="E66" s="24"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="25">
+        <v>3</v>
+      </c>
+      <c r="H66" s="18">
+        <v>17196</v>
+      </c>
+      <c r="I66" s="13">
+        <v>3</v>
+      </c>
       <c r="J66"/>
       <c r="K66"/>
       <c r="L66"/>
@@ -8203,15 +7346,26 @@
       <c r="S66"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="2:20">
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="D67"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
+    <row r="67" spans="1:20">
+      <c r="A67" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13">
+        <v>3810</v>
+      </c>
+      <c r="E67" s="24"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="25">
+        <v>1</v>
+      </c>
+      <c r="H67" s="18">
+        <v>3810</v>
+      </c>
+      <c r="I67" s="13">
+        <v>1</v>
+      </c>
       <c r="J67"/>
       <c r="K67"/>
       <c r="L67"/>
@@ -8224,15 +7378,30 @@
       <c r="S67"/>
       <c r="T67"/>
     </row>
-    <row r="68" spans="2:20">
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="D68"/>
-      <c r="E68"/>
-      <c r="F68"/>
-      <c r="G68"/>
-      <c r="H68"/>
-      <c r="I68"/>
+    <row r="68" spans="1:20">
+      <c r="A68" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13">
+        <v>18426</v>
+      </c>
+      <c r="D68" s="13">
+        <v>54966</v>
+      </c>
+      <c r="E68" s="24"/>
+      <c r="F68" s="25">
+        <v>4</v>
+      </c>
+      <c r="G68" s="25">
+        <v>8</v>
+      </c>
+      <c r="H68" s="18">
+        <v>73392</v>
+      </c>
+      <c r="I68" s="13">
+        <v>12</v>
+      </c>
       <c r="J68"/>
       <c r="K68"/>
       <c r="L68"/>
@@ -8245,15 +7414,30 @@
       <c r="S68"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="2:20">
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="D69"/>
-      <c r="E69"/>
-      <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
+    <row r="69" spans="1:20">
+      <c r="A69" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13">
+        <v>18426</v>
+      </c>
+      <c r="D69" s="13">
+        <v>54966</v>
+      </c>
+      <c r="E69" s="24"/>
+      <c r="F69" s="25">
+        <v>4</v>
+      </c>
+      <c r="G69" s="25">
+        <v>8</v>
+      </c>
+      <c r="H69" s="18">
+        <v>73392</v>
+      </c>
+      <c r="I69" s="13">
+        <v>12</v>
+      </c>
       <c r="J69"/>
       <c r="K69"/>
       <c r="L69"/>
@@ -8266,15 +7450,30 @@
       <c r="S69"/>
       <c r="T69"/>
     </row>
-    <row r="70" spans="2:20">
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
-      <c r="F70"/>
-      <c r="G70"/>
-      <c r="H70"/>
-      <c r="I70"/>
+    <row r="70" spans="1:20">
+      <c r="A70" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13">
+        <v>9552</v>
+      </c>
+      <c r="D70" s="13">
+        <v>33306</v>
+      </c>
+      <c r="E70" s="24"/>
+      <c r="F70" s="25">
+        <v>2</v>
+      </c>
+      <c r="G70" s="25">
+        <v>7</v>
+      </c>
+      <c r="H70" s="18">
+        <v>42858</v>
+      </c>
+      <c r="I70" s="13">
+        <v>9</v>
+      </c>
       <c r="J70"/>
       <c r="K70"/>
       <c r="L70"/>
@@ -8287,15 +7486,30 @@
       <c r="S70"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="2:20">
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
+    <row r="71" spans="1:20">
+      <c r="A71" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13">
+        <v>8874</v>
+      </c>
+      <c r="D71" s="13">
+        <v>21660</v>
+      </c>
+      <c r="E71" s="24"/>
+      <c r="F71" s="25">
+        <v>2</v>
+      </c>
+      <c r="G71" s="25">
+        <v>1</v>
+      </c>
+      <c r="H71" s="18">
+        <v>30534</v>
+      </c>
+      <c r="I71" s="13">
+        <v>3</v>
+      </c>
       <c r="J71"/>
       <c r="K71"/>
       <c r="L71"/>
@@ -8308,15 +7522,34 @@
       <c r="S71"/>
       <c r="T71"/>
     </row>
-    <row r="72" spans="2:20">
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="D72"/>
-      <c r="E72"/>
-      <c r="F72"/>
-      <c r="G72"/>
-      <c r="H72"/>
-      <c r="I72"/>
+    <row r="72" spans="1:20">
+      <c r="A72" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" s="13">
+        <v>6732</v>
+      </c>
+      <c r="C72" s="13">
+        <v>7413</v>
+      </c>
+      <c r="D72" s="13">
+        <v>74589</v>
+      </c>
+      <c r="E72" s="24">
+        <v>3</v>
+      </c>
+      <c r="F72" s="25">
+        <v>2</v>
+      </c>
+      <c r="G72" s="25">
+        <v>9</v>
+      </c>
+      <c r="H72" s="18">
+        <v>88734</v>
+      </c>
+      <c r="I72" s="13">
+        <v>14</v>
+      </c>
       <c r="J72"/>
       <c r="K72"/>
       <c r="L72"/>
@@ -8329,15 +7562,30 @@
       <c r="S72"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="2:20">
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="D73"/>
-      <c r="E73"/>
-      <c r="F73"/>
-      <c r="G73"/>
-      <c r="H73"/>
-      <c r="I73"/>
+    <row r="73" spans="1:20">
+      <c r="A73" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="13">
+        <v>4047</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13">
+        <v>14445</v>
+      </c>
+      <c r="E73" s="24">
+        <v>1</v>
+      </c>
+      <c r="F73" s="25"/>
+      <c r="G73" s="25">
+        <v>4</v>
+      </c>
+      <c r="H73" s="18">
+        <v>18492</v>
+      </c>
+      <c r="I73" s="13">
+        <v>5</v>
+      </c>
       <c r="J73"/>
       <c r="K73"/>
       <c r="L73"/>
@@ -8350,15 +7598,30 @@
       <c r="S73"/>
       <c r="T73"/>
     </row>
-    <row r="74" spans="2:20">
-      <c r="B74"/>
-      <c r="C74"/>
-      <c r="D74"/>
-      <c r="E74"/>
-      <c r="F74"/>
-      <c r="G74"/>
-      <c r="H74"/>
-      <c r="I74"/>
+    <row r="74" spans="1:20">
+      <c r="A74" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B74" s="13">
+        <v>4047</v>
+      </c>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13">
+        <v>14445</v>
+      </c>
+      <c r="E74" s="24">
+        <v>1</v>
+      </c>
+      <c r="F74" s="25"/>
+      <c r="G74" s="25">
+        <v>4</v>
+      </c>
+      <c r="H74" s="18">
+        <v>18492</v>
+      </c>
+      <c r="I74" s="13">
+        <v>5</v>
+      </c>
       <c r="J74"/>
       <c r="K74"/>
       <c r="L74"/>
@@ -8371,15 +7634,30 @@
       <c r="S74"/>
       <c r="T74"/>
     </row>
-    <row r="75" spans="2:20">
-      <c r="B75"/>
-      <c r="C75"/>
-      <c r="D75"/>
-      <c r="E75"/>
-      <c r="F75"/>
-      <c r="G75"/>
-      <c r="H75"/>
-      <c r="I75"/>
+    <row r="75" spans="1:20">
+      <c r="A75" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" s="13">
+        <v>4047</v>
+      </c>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13">
+        <v>14445</v>
+      </c>
+      <c r="E75" s="24">
+        <v>1</v>
+      </c>
+      <c r="F75" s="25"/>
+      <c r="G75" s="25">
+        <v>4</v>
+      </c>
+      <c r="H75" s="18">
+        <v>18492</v>
+      </c>
+      <c r="I75" s="13">
+        <v>5</v>
+      </c>
       <c r="J75"/>
       <c r="K75"/>
       <c r="L75"/>
@@ -8392,15 +7670,34 @@
       <c r="S75"/>
       <c r="T75"/>
     </row>
-    <row r="76" spans="2:20">
-      <c r="B76"/>
-      <c r="C76"/>
-      <c r="D76"/>
-      <c r="E76"/>
-      <c r="F76"/>
-      <c r="G76"/>
-      <c r="H76"/>
-      <c r="I76"/>
+    <row r="76" spans="1:20">
+      <c r="A76" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B76" s="13">
+        <v>2685</v>
+      </c>
+      <c r="C76" s="13">
+        <v>7413</v>
+      </c>
+      <c r="D76" s="13">
+        <v>60144</v>
+      </c>
+      <c r="E76" s="24">
+        <v>2</v>
+      </c>
+      <c r="F76" s="25">
+        <v>2</v>
+      </c>
+      <c r="G76" s="25">
+        <v>5</v>
+      </c>
+      <c r="H76" s="18">
+        <v>70242</v>
+      </c>
+      <c r="I76" s="13">
+        <v>9</v>
+      </c>
       <c r="J76"/>
       <c r="K76"/>
       <c r="L76"/>
@@ -8413,15 +7710,30 @@
       <c r="S76"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="2:20">
-      <c r="B77"/>
-      <c r="C77"/>
-      <c r="D77"/>
-      <c r="E77"/>
-      <c r="F77"/>
-      <c r="G77"/>
-      <c r="H77"/>
-      <c r="I77"/>
+    <row r="77" spans="1:20">
+      <c r="A77" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B77" s="13">
+        <v>2685</v>
+      </c>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13">
+        <v>38193</v>
+      </c>
+      <c r="E77" s="24">
+        <v>2</v>
+      </c>
+      <c r="F77" s="25"/>
+      <c r="G77" s="25">
+        <v>2</v>
+      </c>
+      <c r="H77" s="18">
+        <v>40878</v>
+      </c>
+      <c r="I77" s="13">
+        <v>4</v>
+      </c>
       <c r="J77"/>
       <c r="K77"/>
       <c r="L77"/>
@@ -8434,15 +7746,30 @@
       <c r="S77"/>
       <c r="T77"/>
     </row>
-    <row r="78" spans="2:20">
-      <c r="B78"/>
-      <c r="C78"/>
-      <c r="D78"/>
-      <c r="E78"/>
-      <c r="F78"/>
-      <c r="G78"/>
-      <c r="H78"/>
-      <c r="I78"/>
+    <row r="78" spans="1:20">
+      <c r="A78" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13">
+        <v>7413</v>
+      </c>
+      <c r="D78" s="13">
+        <v>21951</v>
+      </c>
+      <c r="E78" s="24"/>
+      <c r="F78" s="25">
+        <v>2</v>
+      </c>
+      <c r="G78" s="25">
+        <v>3</v>
+      </c>
+      <c r="H78" s="18">
+        <v>29364</v>
+      </c>
+      <c r="I78" s="13">
+        <v>5</v>
+      </c>
       <c r="J78"/>
       <c r="K78"/>
       <c r="L78"/>
@@ -8455,15 +7782,30 @@
       <c r="S78"/>
       <c r="T78"/>
     </row>
-    <row r="79" spans="2:20">
-      <c r="B79"/>
-      <c r="C79"/>
-      <c r="D79"/>
-      <c r="E79"/>
-      <c r="F79"/>
-      <c r="G79"/>
-      <c r="H79"/>
-      <c r="I79"/>
+    <row r="79" spans="1:20">
+      <c r="A79" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13">
+        <v>3633</v>
+      </c>
+      <c r="D79" s="13">
+        <v>21951</v>
+      </c>
+      <c r="E79" s="24"/>
+      <c r="F79" s="25">
+        <v>1</v>
+      </c>
+      <c r="G79" s="25">
+        <v>3</v>
+      </c>
+      <c r="H79" s="18">
+        <v>25584</v>
+      </c>
+      <c r="I79" s="13">
+        <v>4</v>
+      </c>
       <c r="J79"/>
       <c r="K79"/>
       <c r="L79"/>
@@ -8476,15 +7818,26 @@
       <c r="S79"/>
       <c r="T79"/>
     </row>
-    <row r="80" spans="2:20">
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="D80"/>
-      <c r="E80"/>
-      <c r="F80"/>
-      <c r="G80"/>
-      <c r="H80"/>
-      <c r="I80"/>
+    <row r="80" spans="1:20">
+      <c r="A80" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13">
+        <v>3780</v>
+      </c>
+      <c r="D80" s="13"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="25">
+        <v>1</v>
+      </c>
+      <c r="G80" s="25"/>
+      <c r="H80" s="18">
+        <v>3780</v>
+      </c>
+      <c r="I80" s="13">
+        <v>1</v>
+      </c>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80"/>
@@ -8497,15 +7850,34 @@
       <c r="S80"/>
       <c r="T80"/>
     </row>
-    <row r="81" spans="2:20">
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
-      <c r="I81"/>
+    <row r="81" spans="1:20">
+      <c r="A81" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B81" s="13">
+        <v>10023</v>
+      </c>
+      <c r="C81" s="13">
+        <v>169950</v>
+      </c>
+      <c r="D81" s="13">
+        <v>337206</v>
+      </c>
+      <c r="E81" s="24">
+        <v>5</v>
+      </c>
+      <c r="F81" s="25">
+        <v>37</v>
+      </c>
+      <c r="G81" s="25">
+        <v>55</v>
+      </c>
+      <c r="H81" s="18">
+        <v>517179</v>
+      </c>
+      <c r="I81" s="13">
+        <v>97</v>
+      </c>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81"/>
@@ -8518,7 +7890,7 @@
       <c r="S81"/>
       <c r="T81"/>
     </row>
-    <row r="82" spans="2:20">
+    <row r="82" spans="1:20">
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
@@ -8539,7 +7911,7 @@
       <c r="S82"/>
       <c r="T82"/>
     </row>
-    <row r="83" spans="2:20">
+    <row r="83" spans="1:20">
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
@@ -8560,7 +7932,7 @@
       <c r="S83"/>
       <c r="T83"/>
     </row>
-    <row r="84" spans="2:20">
+    <row r="84" spans="1:20">
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
@@ -8581,7 +7953,7 @@
       <c r="S84"/>
       <c r="T84"/>
     </row>
-    <row r="85" spans="2:20">
+    <row r="85" spans="1:20">
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
@@ -8602,7 +7974,7 @@
       <c r="S85"/>
       <c r="T85"/>
     </row>
-    <row r="86" spans="2:20">
+    <row r="86" spans="1:20">
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
@@ -8623,7 +7995,7 @@
       <c r="S86"/>
       <c r="T86"/>
     </row>
-    <row r="87" spans="2:20">
+    <row r="87" spans="1:20">
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
@@ -8644,7 +8016,7 @@
       <c r="S87"/>
       <c r="T87"/>
     </row>
-    <row r="88" spans="2:20">
+    <row r="88" spans="1:20">
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
@@ -8665,7 +8037,7 @@
       <c r="S88"/>
       <c r="T88"/>
     </row>
-    <row r="89" spans="2:20">
+    <row r="89" spans="1:20">
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
@@ -8686,7 +8058,7 @@
       <c r="S89"/>
       <c r="T89"/>
     </row>
-    <row r="90" spans="2:20">
+    <row r="90" spans="1:20">
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
@@ -8707,7 +8079,7 @@
       <c r="S90"/>
       <c r="T90"/>
     </row>
-    <row r="91" spans="2:20">
+    <row r="91" spans="1:20">
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
@@ -8728,7 +8100,7 @@
       <c r="S91"/>
       <c r="T91"/>
     </row>
-    <row r="92" spans="2:20">
+    <row r="92" spans="1:20">
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
@@ -8749,7 +8121,7 @@
       <c r="S92"/>
       <c r="T92"/>
     </row>
-    <row r="93" spans="2:20">
+    <row r="93" spans="1:20">
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
@@ -8770,7 +8142,7 @@
       <c r="S93"/>
       <c r="T93"/>
     </row>
-    <row r="94" spans="2:20">
+    <row r="94" spans="1:20">
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
@@ -8791,7 +8163,7 @@
       <c r="S94"/>
       <c r="T94"/>
     </row>
-    <row r="95" spans="2:20">
+    <row r="95" spans="1:20">
       <c r="B95"/>
       <c r="C95"/>
       <c r="D95"/>
@@ -8812,7 +8184,7 @@
       <c r="S95"/>
       <c r="T95"/>
     </row>
-    <row r="96" spans="2:20">
+    <row r="96" spans="1:20">
       <c r="B96"/>
       <c r="C96"/>
       <c r="D96"/>

</xml_diff>